<commit_message>
masking effect, print more
</commit_message>
<xml_diff>
--- a/project/1st result.xlsx
+++ b/project/1st result.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
   <si>
     <t>lstm1_den_relu_pre_adam_cat</t>
   </si>
@@ -67,15 +67,19 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>is this</t>
+    <t>is this(0.5241)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>what color</t>
+    <t>what is(0.0156)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>what is</t>
+    <t>what color(0.17595)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>is this+what color+what is</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1243,6 +1247,82 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="8747760" y="6179820"/>
+          <a:ext cx="5559070" cy="2988000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>423190</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>122880</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="그림 7"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8755380" y="9288780"/>
+          <a:ext cx="5559070" cy="2988000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>15240</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>209830</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>122880</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="그림 8"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3177540" y="9288780"/>
           <a:ext cx="5559070" cy="2988000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1696,10 +1776,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:A9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -1729,12 +1809,17 @@
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A9" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change batch, learning rate
</commit_message>
<xml_diff>
--- a/project/1st result.xlsx
+++ b/project/1st result.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
   <si>
     <t>lstm1_den_relu_pre_adam_cat</t>
   </si>
@@ -82,6 +82,14 @@
     <t>is this+what color+what is</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>jzs1_m_den_relu_time_soft_pre_adam_cat</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>jzs1_m_den_relu_time_soft_pre_adam_cat_32_0.01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -1184,31 +1192,183 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>7620</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>213360</xdr:rowOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>202210</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>115260</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="그림 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3169920" y="9281160"/>
+          <a:ext cx="5559070" cy="2988000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>220980</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>415570</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>115260</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="그림 6"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8747760" y="9281160"/>
+          <a:ext cx="5559070" cy="2988000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>423190</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>130500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="그림 7"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8755380" y="12390120"/>
+          <a:ext cx="5559070" cy="2988000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>15240</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>209830</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>130500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="그림 8"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3177540" y="12390120"/>
+          <a:ext cx="5559070" cy="2988000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>202210</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>107640</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="그림 5"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3169920" y="6179820"/>
+      <xdr:rowOff>122880</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="그림 9"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3169920" y="6195060"/>
           <a:ext cx="5559070" cy="2988000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1222,107 +1382,31 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>220980</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>213360</xdr:rowOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>415570</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>107640</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="그림 6"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8747760" y="6179820"/>
-          <a:ext cx="5559070" cy="2988000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>423190</xdr:colOff>
-      <xdr:row>55</xdr:row>
       <xdr:rowOff>122880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="그림 7"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8755380" y="9288780"/>
-          <a:ext cx="5559070" cy="2988000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>15240</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>209830</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>122880</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="9" name="그림 8"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3177540" y="9288780"/>
+        <xdr:cNvPr id="11" name="그림 10"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8747760" y="6195060"/>
           <a:ext cx="5559070" cy="2988000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1776,7 +1860,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A9"/>
+  <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
@@ -1802,6 +1886,11 @@
         <v>13</v>
       </c>
     </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+    </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>13</v>
@@ -1820,6 +1909,11 @@
     <row r="9" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A11" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change batch size, use fit
</commit_message>
<xml_diff>
--- a/project/1st result.xlsx
+++ b/project/1st result.xlsx
@@ -9,15 +9,15 @@
   <sheets>
     <sheet name="is this_all" sheetId="1" r:id="rId1"/>
     <sheet name="is this_select" sheetId="2" r:id="rId2"/>
-    <sheet name="what color" sheetId="3" r:id="rId3"/>
-    <sheet name="jzs1" sheetId="4" r:id="rId4"/>
+    <sheet name="jzs1" sheetId="4" r:id="rId3"/>
+    <sheet name="여기부터 fit" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="35">
   <si>
     <t>lstm1_den_relu_pre_adam_cat</t>
   </si>
@@ -55,10 +55,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>lstm2_den_soft_pre_adam_cat</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>jzs1_den_relu_time_soft_pre_adam_cat</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -79,15 +75,78 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>jzs1_m_den_relu_time_soft_pre_adam_cat</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>jzs1_m_den_relu_time_soft_pre_adam_cat_32_0.01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>is this+what color+what is(0.1752)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>jzs1_m_den_relu_time_soft_pre_adam_cat_32_0.1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>jzs1_m_den_relu_time_soft_pre_adam_cat</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fit으로 바꾸기. Val 넣어서</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>그래프 같이 그리고</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>simpleRNN에서 default/identity, lstm, jzs1 바꿔가면서 해보고</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>batchsize=1 2 4 8 16 32</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>단어들 빈도수 찍어서 적으면 unknown 토큰.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>multi-bleu 스코어 cost???</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>text qa 모델 설명. One hot 코딩해서… embedding layer 거쳐서.. Time step별로 네트워크 펼쳐서… eof 나오면.. Answer가 나와서.. 단어가 생성됨…</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>what is</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>is this+what color+what is</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>jzs1_m_den_relu_time_soft_pre_adam_cat</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>jzs1_m_den_relu_time_soft_pre_adam_cat_32_0.01</t>
+    <t>jzs1_embed_den_relu_time_soft_pre_adam_cat</t>
+  </si>
+  <si>
+    <t>jzs1_embed_den_relu_time_soft_pre_adam_cat</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lstm_embed_den_relu_time_soft_pre_adam_cat</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>발표는..</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>jzs1_embed_den_relu_time_soft_post_adam_cat</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -95,7 +154,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -105,6 +164,15 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
@@ -131,8 +199,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -1038,16 +1107,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>7621</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>3154681</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>13240</xdr:rowOff>
+      <xdr:rowOff>22860</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>202212</xdr:colOff>
+      <xdr:colOff>186972</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>128500</xdr:rowOff>
+      <xdr:rowOff>138120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1064,7 +1133,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3169921" y="13240"/>
+          <a:off x="3154681" y="22860"/>
           <a:ext cx="5559071" cy="2988000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1407,6 +1476,386 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="8747760" y="6195060"/>
+          <a:ext cx="5559070" cy="2988000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>194590</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>115260</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="그림 11"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3162300" y="15468600"/>
+          <a:ext cx="5559070" cy="2988000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>423190</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>115260</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="그림 12"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8755380" y="15468600"/>
+          <a:ext cx="5559070" cy="2988000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>228601</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>423191</xdr:colOff>
+      <xdr:row>97</xdr:row>
+      <xdr:rowOff>122880</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="그림 13"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8755381" y="18569940"/>
+          <a:ext cx="5559070" cy="2988000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>194590</xdr:colOff>
+      <xdr:row>97</xdr:row>
+      <xdr:rowOff>115260</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="그림 14"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3162300" y="18562320"/>
+          <a:ext cx="5559070" cy="2988000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>98</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>202210</xdr:colOff>
+      <xdr:row>111</xdr:row>
+      <xdr:rowOff>122880</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="그림 15"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3169920" y="21663660"/>
+          <a:ext cx="5559070" cy="2988000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>243840</xdr:colOff>
+      <xdr:row>98</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>438430</xdr:colOff>
+      <xdr:row>111</xdr:row>
+      <xdr:rowOff>115260</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="그림 16"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8770620" y="21656040"/>
+          <a:ext cx="5559070" cy="2988000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>243840</xdr:colOff>
+      <xdr:row>112</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>438430</xdr:colOff>
+      <xdr:row>125</xdr:row>
+      <xdr:rowOff>115260</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="그림 17"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8770620" y="24749760"/>
+          <a:ext cx="5559070" cy="2988000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>112</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>194590</xdr:colOff>
+      <xdr:row>125</xdr:row>
+      <xdr:rowOff>115260</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="그림 18"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3162300" y="24749760"/>
+          <a:ext cx="5559070" cy="2988000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>126</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>193920</xdr:colOff>
+      <xdr:row>139</xdr:row>
+      <xdr:rowOff>115260</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="그림 20"/>
+        <xdr:cNvPicPr>
+          <a:picLocks/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3162300" y="27843480"/>
+          <a:ext cx="5558400" cy="2988000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>243840</xdr:colOff>
+      <xdr:row>126</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>438430</xdr:colOff>
+      <xdr:row>139</xdr:row>
+      <xdr:rowOff>122880</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="22" name="그림 21"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8770620" y="27851100"/>
           <a:ext cx="5559070" cy="2988000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1709,7 +2158,7 @@
   <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -1733,37 +2182,37 @@
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A8" t="s">
+      <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A9" t="s">
+      <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A10" t="s">
+      <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1832,38 +2281,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A19"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
-  <cols>
-    <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A11"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -1873,47 +2294,77 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
-        <v>13</v>
+      <c r="A3" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A4" t="s">
-        <v>18</v>
+      <c r="A4" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A7" t="s">
-        <v>16</v>
+      <c r="A7" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A8" t="s">
-        <v>15</v>
+      <c r="A8" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A18" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A19" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1922,4 +2373,79 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="45.69921875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="B6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="B7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="B8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>